<commit_message>
Atualizado com as novas informações de distribuição
</commit_message>
<xml_diff>
--- a/IronBBQ_v08.xlsx
+++ b/IronBBQ_v08.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Pessoas" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,67 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Path, Charles</author>
+  </authors>
+  <commentList>
+    <comment ref="L17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path, Charles:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fabio?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path, Charles:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Fabio tem uma loja perto da casa, consegue pegar?
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="116">
   <si>
     <t>Charles</t>
   </si>
@@ -368,6 +427,12 @@
   </si>
   <si>
     <t>Picolés</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>173,57</t>
   </si>
 </sst>
 </file>
@@ -377,7 +442,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,8 +465,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +510,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -744,7 +846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -860,6 +962,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1175,10 +1290,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1305,7 @@
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
@@ -1213,7 +1328,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1233,10 +1348,10 @@
       </c>
       <c r="G2" s="49">
         <f>(C2+E2)*QuantidadeEValores!$C$37</f>
-        <v>57.857916666666675</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63.117727272727279</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1259,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1279,10 +1394,10 @@
       </c>
       <c r="G4" s="49">
         <f>(C4+E4)*QuantidadeEValores!$C$37</f>
-        <v>115.71583333333335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126.23545454545456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1304,10 +1419,10 @@
       </c>
       <c r="G5" s="49">
         <f>(C5+E5)*QuantidadeEValores!$C$37</f>
-        <v>231.4316666666667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>252.47090909090912</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1329,18 +1444,18 @@
       </c>
       <c r="G6" s="49">
         <f>(C6+E6)*QuantidadeEValores!$C$37</f>
-        <v>173.57375000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189.35318181818184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
@@ -1352,10 +1467,10 @@
       </c>
       <c r="G7" s="49">
         <f>(C7+E7)*QuantidadeEValores!$C$37</f>
-        <v>115.71583333333335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1377,10 +1492,10 @@
       </c>
       <c r="G8" s="49">
         <f>(C8+E8)*QuantidadeEValores!$C$37</f>
-        <v>173.57375000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189.35318181818184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1402,10 +1517,16 @@
       </c>
       <c r="G9" s="49">
         <f>(C9+E9)*QuantidadeEValores!$C$37</f>
-        <v>173.57375000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>189.35318181818184</v>
+      </c>
+      <c r="H9" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1425,10 +1546,16 @@
       </c>
       <c r="G10" s="49">
         <f>(C10+E10)*QuantidadeEValores!$C$37</f>
-        <v>115.71583333333335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126.23545454545456</v>
+      </c>
+      <c r="H10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1448,10 +1575,10 @@
       </c>
       <c r="G11" s="49">
         <f>(C11+E11)*QuantidadeEValores!$C$37</f>
-        <v>115.71583333333335</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126.23545454545456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -1473,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1493,10 +1620,10 @@
       </c>
       <c r="G13" s="49">
         <f>(C13+E13)*QuantidadeEValores!$C$37</f>
-        <v>115.71583333333335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126.23545454545456</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1513,17 +1640,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
       <c r="B15" s="1">
         <f>SUM(B2:B14)</f>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <f>SUM(C2:C14)</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D15">
         <f>SUM(D2:D14)</f>
@@ -1540,7 +1667,7 @@
       </c>
       <c r="B17" s="1">
         <f>C15+E15</f>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1563,7 +1690,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="2" bestFit="1" customWidth="1"/>
@@ -2042,11 +2171,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2184,7 @@
     <col min="3" max="3" width="19.140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="6" max="6" width="18.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="12" max="12" width="20.140625" customWidth="1"/>
     <col min="13" max="14" width="14.140625" customWidth="1"/>
@@ -2077,14 +2206,14 @@
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="53">
         <f>Pessoas!B17</f>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="30">
         <v>400</v>
       </c>
       <c r="D3" s="31">
         <f>B3*C3/1000</f>
-        <v>9.6</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
@@ -2142,7 +2271,7 @@
       </c>
       <c r="C11" s="44">
         <f>D3-D9</f>
-        <v>5.0999999999999996</v>
+        <v>4.3000000000000007</v>
       </c>
       <c r="F11" s="27"/>
     </row>
@@ -2209,316 +2338,316 @@
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="63">
         <v>5</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="29">
+      <c r="E16" s="64">
         <f>C16*Valores!J5</f>
         <v>119.9</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="28">
-        <v>2</v>
-      </c>
-      <c r="I16" s="28" t="s">
+      <c r="H16" s="66">
+        <v>2</v>
+      </c>
+      <c r="I16" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="J16" s="29">
+      <c r="J16" s="67">
         <f>H16*Valores!B15</f>
         <v>5</v>
       </c>
-      <c r="L16" s="7" t="s">
+      <c r="L16" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="M16" s="28">
-        <v>2</v>
-      </c>
-      <c r="N16" s="51" t="s">
+      <c r="M16" s="66">
+        <v>2</v>
+      </c>
+      <c r="N16" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="O16" s="29" t="s">
+      <c r="O16" s="67" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="63">
         <f>G9</f>
         <v>2.25</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="29">
+      <c r="E17" s="64">
         <f>C17*Valores!I10</f>
         <v>74.25</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="66">
         <v>500</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="29">
+      <c r="J17" s="67">
         <f>H17/1000*Valores!B16</f>
         <v>1.25</v>
       </c>
-      <c r="L17" s="7" t="s">
+      <c r="L17" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="M17" s="28">
+      <c r="M17" s="70">
         <v>1</v>
       </c>
-      <c r="N17" s="51" t="s">
+      <c r="N17" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="O17" s="29">
+      <c r="O17" s="71">
         <f>M17*Valores!B29</f>
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="63">
         <v>3</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E18" s="29">
+      <c r="E18" s="64">
         <f>C18*Valores!I4</f>
         <v>119.69999999999999</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="63">
         <v>1</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="J18" s="29">
+      <c r="J18" s="64">
         <f>H18*Valores!B17</f>
         <v>25</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L18" s="69" t="s">
         <v>88</v>
       </c>
-      <c r="M18" s="28">
+      <c r="M18" s="70">
         <v>1</v>
       </c>
-      <c r="N18" s="51" t="s">
+      <c r="N18" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="O18" s="29">
+      <c r="O18" s="71">
         <f>M18*Valores!B30</f>
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="63">
         <v>1</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="29">
+      <c r="E19" s="64">
         <f>C19*Valores!I7</f>
         <v>14.99</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="28">
+      <c r="H19" s="66">
         <v>4</v>
       </c>
-      <c r="I19" s="28" t="s">
+      <c r="I19" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="J19" s="29">
+      <c r="J19" s="67">
         <f>H19*Valores!B18</f>
         <v>20</v>
       </c>
-      <c r="L19" s="7" t="s">
+      <c r="L19" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="M19" s="28">
-        <v>2</v>
-      </c>
-      <c r="N19" s="51" t="s">
+      <c r="M19" s="70">
+        <v>2</v>
+      </c>
+      <c r="N19" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="O19" s="29">
+      <c r="O19" s="71">
         <f>M19*Valores!B31</f>
         <v>4</v>
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="28">
-        <v>2</v>
-      </c>
-      <c r="D20" s="28" t="s">
+      <c r="C20" s="63">
+        <v>2</v>
+      </c>
+      <c r="D20" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E20" s="64">
         <f>C20*Valores!I13</f>
         <v>11.96</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20" s="66">
         <v>5</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="J20" s="29">
+      <c r="J20" s="67">
         <f>H20*Valores!B19</f>
         <v>34.5</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="L20" s="69" t="s">
         <v>90</v>
       </c>
-      <c r="M20" s="28">
+      <c r="M20" s="70">
         <v>5</v>
       </c>
-      <c r="N20" s="51" t="s">
+      <c r="N20" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="O20" s="29">
+      <c r="O20" s="71">
         <f>M20*Valores!B32</f>
         <v>10</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="28">
-        <v>2</v>
-      </c>
-      <c r="D21" s="28" t="s">
+      <c r="C21" s="63">
+        <v>2</v>
+      </c>
+      <c r="D21" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="29">
+      <c r="E21" s="64">
         <f>C21*Valores!I3</f>
         <v>49.8</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="H21" s="28">
+      <c r="H21" s="66">
         <v>1</v>
       </c>
-      <c r="I21" s="28" t="s">
+      <c r="I21" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="J21" s="29">
+      <c r="J21" s="67">
         <f>H21*Valores!B20</f>
         <v>10</v>
       </c>
-      <c r="L21" s="7" t="s">
+      <c r="L21" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="M21" s="28">
-        <v>2</v>
-      </c>
-      <c r="N21" s="51" t="s">
+      <c r="M21" s="66">
+        <v>2</v>
+      </c>
+      <c r="N21" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="O21" s="29">
+      <c r="O21" s="67">
         <f>M21*Valores!B27</f>
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="28">
-        <v>2</v>
-      </c>
-      <c r="D22" s="28" t="s">
+      <c r="C22" s="63">
+        <v>2</v>
+      </c>
+      <c r="D22" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="29">
+      <c r="E22" s="64">
         <f>C22*Valores!I12</f>
         <v>31.8</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="H22" s="28">
-        <v>2</v>
-      </c>
-      <c r="I22" s="28" t="s">
+      <c r="H22" s="63">
+        <v>2</v>
+      </c>
+      <c r="I22" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="J22" s="29">
+      <c r="J22" s="64">
         <f>H22*Valores!B21</f>
         <v>12</v>
       </c>
-      <c r="L22" s="7" t="s">
+      <c r="L22" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="M22" s="28">
+      <c r="M22" s="63">
         <v>3</v>
       </c>
-      <c r="N22" s="51" t="s">
+      <c r="N22" s="65" t="s">
         <v>111</v>
       </c>
-      <c r="O22" s="29">
+      <c r="O22" s="64">
         <f>M22*Valores!B28</f>
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="63">
         <v>4</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="E23" s="29">
+      <c r="E23" s="64">
         <f>C23*Valores!I8</f>
         <v>35.6</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="H23" s="28">
+      <c r="H23" s="66">
         <v>3</v>
       </c>
-      <c r="I23" s="28" t="s">
+      <c r="I23" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="J23" s="29">
+      <c r="J23" s="67">
         <f>H23*Valores!B22</f>
         <v>15</v>
       </c>
@@ -2528,29 +2657,29 @@
       <c r="O23" s="29"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="63">
         <v>3</v>
       </c>
-      <c r="D24" s="28" t="s">
+      <c r="D24" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="64">
         <f>C24*Valores!D9</f>
         <v>137.69999999999999</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="63">
         <v>1</v>
       </c>
-      <c r="I24" s="28" t="s">
+      <c r="I24" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24" s="64">
         <f>H24*Valores!B23</f>
         <v>2.9</v>
       </c>
@@ -2564,16 +2693,16 @@
       <c r="C25" s="28"/>
       <c r="D25" s="28"/>
       <c r="E25" s="29"/>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="H25" s="28">
+      <c r="H25" s="70">
         <v>72</v>
       </c>
-      <c r="I25" s="28" t="s">
+      <c r="I25" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="71">
         <v>1</v>
       </c>
       <c r="L25" s="7"/>
@@ -2586,16 +2715,16 @@
       <c r="C26" s="28"/>
       <c r="D26" s="28"/>
       <c r="E26" s="29"/>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="H26" s="28">
+      <c r="H26" s="63">
         <v>27</v>
       </c>
-      <c r="I26" s="28" t="s">
+      <c r="I26" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26" s="64">
         <f>H26*Valores!B24</f>
         <v>3.2399999999999998</v>
       </c>
@@ -2698,7 +2827,7 @@
       </c>
       <c r="C37" s="49">
         <f>C36/Pessoas!B17</f>
-        <v>57.857916666666675</v>
+        <v>63.117727272727279</v>
       </c>
     </row>
   </sheetData>
@@ -2709,5 +2838,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>